<commit_message>
Fix tea time demo to use Survey forms
</commit_message>
<xml_diff>
--- a/app/config/tables/Tea_types/forms/Tea_types/Tea_types.xlsx
+++ b/app/config/tables/Tea_types/forms/Tea_types/Tea_types.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/tables/Tea_types/forms/Tea_types/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="5600" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="7040" yWindow="5360" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -17,13 +12,13 @@
     <sheet name="settings" sheetId="3" r:id="rId3"/>
     <sheet name="properties" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -62,12 +57,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>Type_id</t>
-  </si>
-  <si>
-    <t>Enter the Tea Type ID</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -168,6 +157,12 @@
   </si>
   <si>
     <t>key</t>
+  </si>
+  <si>
+    <t>instance_name</t>
+  </si>
+  <si>
+    <t>required</t>
   </si>
 </sst>
 </file>
@@ -242,13 +237,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -306,7 +299,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -341,7 +334,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -518,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -526,15 +519,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
@@ -543,7 +536,7 @@
     <col min="7" max="7" width="59.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,23 +558,25 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
@@ -591,10 +586,16 @@
       <c r="G3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
@@ -602,8 +603,11 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -616,22 +620,19 @@
       <c r="G5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -639,7 +640,7 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -647,7 +648,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -655,7 +656,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -663,7 +664,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -671,7 +672,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -679,7 +680,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -687,7 +688,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -695,25 +696,25 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
+    <row r="16" spans="1:8">
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="2"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="2"/>
+    <row r="18" spans="2:7">
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="2:7">
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -721,7 +722,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7">
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -729,7 +730,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7">
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -737,7 +738,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7">
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -745,7 +746,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7">
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -753,7 +754,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7">
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -761,7 +762,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7">
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -769,7 +770,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7">
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -777,7 +778,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7">
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -785,7 +786,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7">
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -793,7 +794,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7">
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -801,7 +802,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7">
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -809,25 +810,22 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
+    <row r="32" spans="2:7">
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="4:4">
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:4">
       <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -839,104 +837,126 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30">
+      <c r="A6" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="B6" s="4" t="b">
         <v>1</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -948,94 +968,99 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>43</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix properties for Tea_types
</commit_message>
<xml_diff>
--- a/app/config/tables/Tea_types/forms/Tea_types/Tea_types.xlsx
+++ b/app/config/tables/Tea_types/forms/Tea_types/Tea_types.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="5360" windowWidth="26960" windowHeight="15380" tabRatio="500"/>
+    <workbookView xWindow="7040" yWindow="5360" windowWidth="26960" windowHeight="15380" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>comments</t>
   </si>
@@ -124,12 +124,6 @@
   </si>
   <si>
     <t>default</t>
-  </si>
-  <si>
-    <t>colOrder</t>
-  </si>
-  <si>
-    <t>["Type_id","Name","Caffeinated","Origin","Fermented"]</t>
   </si>
   <si>
     <t>defaultViewType</t>
@@ -521,7 +515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
@@ -559,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -944,7 +938,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
@@ -962,23 +956,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1036,23 +1030,6 @@
       </c>
       <c r="E4" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>